<commit_message>
Added getWeekenders to overview, display change in getWeekenders
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA238750-650E-40BF-90D0-9E5C2903868D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0834B233-FB25-4742-8BD3-7273D33CCD07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DA9F082-1D90-46F9-BC45-81B8A7A3A050}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
   <si>
     <t>description</t>
   </si>
@@ -375,6 +375,21 @@
   </si>
   <si>
     <t>2 h</t>
+  </si>
+  <si>
+    <t>getWeekenders.py</t>
+  </si>
+  <si>
+    <t>weekenders.json</t>
+  </si>
+  <si>
+    <t>{"[userID]": {"WD": [numberContributions], "WE": [numberContributions]}, … }</t>
+  </si>
+  <si>
+    <t>{"712": {"WD": 1627, "WE": 524}, … }</t>
+  </si>
+  <si>
+    <t>creates file for number of contributions on weekdays and weekends (in the local timezone) for each user</t>
   </si>
 </sst>
 </file>
@@ -806,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6029F670-A500-4107-B589-0CCEAFD0F2C8}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,6 +1152,29 @@
         <v>77</v>
       </c>
     </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>